<commit_message>
Adjustment to prevent additional coal CCS retrofits beyond EPA projections
</commit_message>
<xml_diff>
--- a/InputData/elec/BBPPRTY/BAU Ban Power Plant Retrofits This Year.xlsx
+++ b/InputData/elec/BBPPRTY/BAU Ban Power Plant Retrofits This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBPPRTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90DEBFF-EF90-4038-9856-5C954E6DA2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE67D9E7-BF42-4CB9-AA54-8F4523DF4DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Source:</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>We do not allow CCS retrofits before 2028, aligned with NREL's approach.</t>
+  </si>
+  <si>
+    <t>We already include all coal CCS retrofits projected by EPA as part of its 111 rules.</t>
+  </si>
+  <si>
+    <t>Projected coal retriements and retrofits cover all of the exisiting coal fleet between</t>
+  </si>
+  <si>
+    <t>2028 and 2035, so we do not allow any additional retrofits.</t>
   </si>
 </sst>
 </file>
@@ -520,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +591,21 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +622,7 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:H22"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,95 +2345,95 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
-        <v>0</v>
-      </c>
-      <c r="M19" s="5">
-        <v>0</v>
-      </c>
-      <c r="N19" s="5">
-        <v>0</v>
-      </c>
-      <c r="O19" s="5">
-        <v>0</v>
-      </c>
-      <c r="P19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>0</v>
-      </c>
-      <c r="R19" s="5">
-        <v>0</v>
-      </c>
-      <c r="S19" s="5">
-        <v>0</v>
-      </c>
-      <c r="T19" s="5">
-        <v>0</v>
-      </c>
-      <c r="U19" s="5">
-        <v>0</v>
-      </c>
-      <c r="V19" s="5">
-        <v>0</v>
-      </c>
-      <c r="W19" s="5">
-        <v>0</v>
-      </c>
-      <c r="X19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="5">
-        <v>0</v>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>